<commit_message>
--appendRowData got created and test
</commit_message>
<xml_diff>
--- a/src/test/java/west/com/OxygenThree/testResult/MISTestResult_2018_04_04_13_28_02.xlsx
+++ b/src/test/java/west/com/OxygenThree/testResult/MISTestResult_2018_04_04_13_28_02.xlsx
@@ -2,28 +2,29 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="10335" windowHeight="3195"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="MISTestResult" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Report Name</t>
+    <t>Call Summary</t>
+  </si>
+  <si>
+    <t>test Result</t>
   </si>
   <si>
     <t>Test Result</t>
-  </si>
-  <si>
-    <t>Pass or Fail</t>
   </si>
 </sst>
 </file>
@@ -33,7 +34,7 @@
   <fonts count="1">
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,12 +358,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -379,4 +383,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>